<commit_message>
Added a setTimeout window.stop  to prevent endless page loading
</commit_message>
<xml_diff>
--- a/myFile.xlsx
+++ b/myFile.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95AC7A3E-C660-41FB-A083-323D3714F31C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="180" windowWidth="20490" windowHeight="10740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="180" windowWidth="20490" windowHeight="10740"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,243 +19,162 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="77">
-  <si>
-    <t>Stealing Home</t>
-  </si>
-  <si>
-    <t>American Graffiti</t>
-  </si>
-  <si>
-    <t>Fried Green Tomatoes</t>
-  </si>
-  <si>
-    <t>Breaking Away</t>
-  </si>
-  <si>
-    <t>Field of Dreams</t>
-  </si>
-  <si>
-    <t>Boyz N the Hood</t>
-  </si>
-  <si>
-    <t>Raising Arizona</t>
-  </si>
-  <si>
-    <t>St. Elmo’s Fire</t>
-  </si>
-  <si>
-    <t>Three Men and a Baby</t>
-  </si>
-  <si>
-    <t>Singles</t>
-  </si>
-  <si>
-    <t>Stand by Me</t>
-  </si>
-  <si>
-    <t>He Said, She Said</t>
-  </si>
-  <si>
-    <t>Home Alone</t>
-  </si>
-  <si>
-    <t>When Harry Met Sally</t>
-  </si>
-  <si>
-    <t>Radio Flyer</t>
-  </si>
-  <si>
-    <t>Little Big Man</t>
-  </si>
-  <si>
-    <t>Heathers</t>
-  </si>
-  <si>
-    <t>Grumpy Old Men</t>
-  </si>
-  <si>
-    <t>Pretty in Pink</t>
-  </si>
-  <si>
-    <t>Parenthood</t>
-  </si>
-  <si>
-    <t>Sixteen Candles</t>
-  </si>
-  <si>
-    <t>Shadowlands</t>
-  </si>
-  <si>
-    <t>Father of the Bride</t>
-  </si>
-  <si>
-    <t>Flatliners</t>
-  </si>
-  <si>
-    <t>The Graduate</t>
-  </si>
-  <si>
-    <t>The Power of One</t>
-  </si>
-  <si>
-    <t>Forrest Gump</t>
-  </si>
-  <si>
-    <t>The World According to Garp</t>
-  </si>
-  <si>
-    <t>My Girl</t>
-  </si>
-  <si>
-    <t>Circle of Friends</t>
-  </si>
-  <si>
-    <t>Muriel’s Wedding</t>
-  </si>
-  <si>
-    <t>Nell</t>
-  </si>
-  <si>
-    <t>A River Runs Through It</t>
-  </si>
-  <si>
-    <t>Life with Father</t>
-  </si>
-  <si>
-    <t>Cocoon</t>
-  </si>
-  <si>
-    <t>Grand Canyon</t>
-  </si>
-  <si>
-    <t>What’s Eating Gilbert Grape</t>
-  </si>
-  <si>
-    <t>Risky Business</t>
-  </si>
-  <si>
-    <t>The Outsiders</t>
-  </si>
-  <si>
-    <t>4 Weddings &amp; a Funeral</t>
-  </si>
-  <si>
-    <t>Wild Strawberries (subtitled)</t>
-  </si>
-  <si>
-    <t>Ran (subtitled)</t>
-  </si>
-  <si>
-    <t>Cinema Paradiso (subtitled)</t>
-  </si>
-  <si>
-    <t>Widow’s Peak</t>
-  </si>
-  <si>
-    <t>Nine Months</t>
-  </si>
-  <si>
-    <t>Jack</t>
-  </si>
-  <si>
-    <t>Wyatt Earp</t>
-  </si>
-  <si>
-    <t>Indian in the Cupboard</t>
-  </si>
-  <si>
-    <t>Dolores Claiborne</t>
-  </si>
-  <si>
-    <t>Grumpier Old Men</t>
-  </si>
-  <si>
-    <t>As Good As It Gets</t>
-  </si>
-  <si>
-    <t>10 Things I Hate About You</t>
-  </si>
-  <si>
-    <t>Never Been Kissed</t>
-  </si>
-  <si>
-    <t>Big Daddy</t>
-  </si>
-  <si>
-    <t>The Wedding Singer</t>
-  </si>
-  <si>
-    <t>Sling Blade</t>
-  </si>
-  <si>
-    <t>The Notebook</t>
-  </si>
-  <si>
-    <t>Bridget Jones's Diary</t>
-  </si>
-  <si>
-    <t>Secondhand Lions</t>
-  </si>
-  <si>
-    <t>Sweet Home Alabama</t>
-  </si>
-  <si>
-    <t>About a Boy</t>
-  </si>
-  <si>
-    <t>Mean Girls</t>
-  </si>
-  <si>
-    <t>A Beautiful Life</t>
-  </si>
-  <si>
-    <t>Something’s Gotta Give</t>
-  </si>
-  <si>
-    <t>The Bucket List</t>
-  </si>
-  <si>
-    <t>Alexander and the Terrible, Horrible, No Good, Very Bad Day</t>
-  </si>
-  <si>
-    <t>The Million Dollar Arm</t>
-  </si>
-  <si>
-    <t>Mom’s Night Out</t>
-  </si>
-  <si>
-    <t>Saving Mr. Banks</t>
-  </si>
-  <si>
-    <t>Parental Guidance</t>
-  </si>
-  <si>
-    <t>Diary of A Wimpy Kid: Dog Days</t>
-  </si>
-  <si>
-    <t>Crazy, Stupid, Love</t>
-  </si>
-  <si>
-    <t>Judy Moody and The Not Bummer Summer</t>
-  </si>
-  <si>
-    <t>Diary of A Wimpy Kid: Roderick Rules</t>
-  </si>
-  <si>
-    <t>Up</t>
-  </si>
-  <si>
-    <t>Real Genius</t>
-  </si>
-  <si>
-    <t>True Grit</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+  <si>
+    <t>Busta Rhymes: "Pass the Courvoisier" Remix</t>
+  </si>
+  <si>
+    <t>David Banner: "Play"</t>
+  </si>
+  <si>
+    <t>Big Boi: "Lookin' 4 Ya" (Ft. Andre 3000 &amp; Sleepy Brown)</t>
+  </si>
+  <si>
+    <t>T.I.: "Big Things Poppin'"</t>
+  </si>
+  <si>
+    <t>GS Boyz: "Stanky Legg"</t>
+  </si>
+  <si>
+    <t>Eve: "Tambourine"</t>
+  </si>
+  <si>
+    <t>Yung Joc: "It's Goin' Down" (Ft. Nitti)</t>
+  </si>
+  <si>
+    <t>Junior M.A.F.I.A.: "Get Money"</t>
+  </si>
+  <si>
+    <t>Azealia Banks: "212"</t>
+  </si>
+  <si>
+    <t>Terror Squad: "Lean Back"</t>
+  </si>
+  <si>
+    <t>Soulja Boy: "Crank Dat (Soulja Boy)"</t>
+  </si>
+  <si>
+    <t>Timbaland: "The Way I Are" (Ft. Keri Hilson &amp; D.O.E.)</t>
+  </si>
+  <si>
+    <t>Chingy: "Right Thurr"</t>
+  </si>
+  <si>
+    <t>A$AP Rocky: "Wild for the Night" (Ft. Skrillex)</t>
+  </si>
+  <si>
+    <t>Jay Z: "I Just Wanna Love U (Give It to Me)"</t>
+  </si>
+  <si>
+    <t>D4L: "Laffy Taffy"</t>
+  </si>
+  <si>
+    <t>Trick Daddy: "Let's Go" (Ft. Lil Jon &amp; Twista)</t>
+  </si>
+  <si>
+    <t>Missy Elliott: "Work It"</t>
+  </si>
+  <si>
+    <t>Hurricane Chris: "A Bay Bay"</t>
+  </si>
+  <si>
+    <t>MC Hammer: "U Can't Touch This"</t>
+  </si>
+  <si>
+    <t>Ludacris: "Stand Up" (Ft. Shawnna)</t>
+  </si>
+  <si>
+    <t>Black Eyed Peas: "I Gotta Feeling"</t>
+  </si>
+  <si>
+    <t>The Cool Kids: "Black Mags"</t>
+  </si>
+  <si>
+    <t>Sage the Gemini: "Gas Pedal"</t>
+  </si>
+  <si>
+    <t>Young Dro: "Shoulder Lean"</t>
+  </si>
+  <si>
+    <t>Cassidy: "My Drink N' My 2-Step"</t>
+  </si>
+  <si>
+    <t>50 Cent: "In da Club"</t>
+  </si>
+  <si>
+    <t>DJ Snake: "Turn Down for What" (Ft. Lil Jon)</t>
+  </si>
+  <si>
+    <t>The Notorious B.I.G.: "Hypnotize"</t>
+  </si>
+  <si>
+    <t>Nelly: "Hot in Herre"</t>
+  </si>
+  <si>
+    <t>Webstar x Young B: "Chicken Noodle Soup"</t>
+  </si>
+  <si>
+    <t>Mystikal: "Shake Ya Ass"</t>
+  </si>
+  <si>
+    <t>Huey: "Pop, Lock &amp; Drop It"</t>
+  </si>
+  <si>
+    <t>N.E.R.D.: "Everyone Nose (All The Girls Standing In The Line For The Bathroom)"</t>
+  </si>
+  <si>
+    <t>Missy Elliott: "Get Ur Freak On"</t>
+  </si>
+  <si>
+    <t>T-Pain: "Buy U a Drank (Shawty Snappin')"</t>
+  </si>
+  <si>
+    <t>Lil Jon and The Eastside Boyz: "Get Low"</t>
+  </si>
+  <si>
+    <t>Unk: "Walk It Out"</t>
+  </si>
+  <si>
+    <t>Dem Franchise Boyz: "Lean Wit It, Rock Wit It"</t>
+  </si>
+  <si>
+    <t>Jim Jones: "We Fly High"</t>
+  </si>
+  <si>
+    <t>Cali Swag District: "Teach Me How to Dougie"</t>
+  </si>
+  <si>
+    <t>C+C Music Factory: "Gonna Make U Sweat (Everybody Dance)"</t>
+  </si>
+  <si>
+    <t>OutKast: "The Way You Move"</t>
+  </si>
+  <si>
+    <t>Missy Elliott: "Lose Control"</t>
+  </si>
+  <si>
+    <t>Flo Rida: "Low"</t>
+  </si>
+  <si>
+    <t>French Montana: "Pop That" (Ft. Drake)</t>
+  </si>
+  <si>
+    <t>OutKast: "Hey Ya!"</t>
+  </si>
+  <si>
+    <t>Snoop Dogg: "Drop It Like It's Hot"</t>
+  </si>
+  <si>
+    <t>Uncle Luke: "I Wanna Rock (Doo Doo Brown)"</t>
+  </si>
+  <si>
+    <t>Rob Base and DJ EZ Rock: "It Takes Two"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -348,7 +266,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -383,7 +301,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -560,18 +478,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A79"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A79"/>
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -829,151 +747,6 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>76</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>